<commit_message>
Add keyboard and audio blocks
</commit_message>
<xml_diff>
--- a/resources/Assembly.xlsx
+++ b/resources/Assembly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\gtxl\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1496BCA-5D8D-4513-AF0F-717B0C953804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBA54D4-52D9-4FFC-975A-E07BC8B27452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="69525" yWindow="-3780" windowWidth="34230" windowHeight="18135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68385" yWindow="-4170" windowWidth="34230" windowHeight="18135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="Z59" sqref="Z59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5666,9 +5666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D4C858-904D-45CD-9444-9CF049B0AF8F}">
   <dimension ref="A1:H258"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Remove timer registers.  Change X register to be the new timer.
</commit_message>
<xml_diff>
--- a/resources/Assembly.xlsx
+++ b/resources/Assembly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\gtxl\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689FFC87-5C0C-4655-AB17-DB0C9080D725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12050C4-81AE-4CF3-BED7-73ED8D1B6C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5505" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="133">
   <si>
     <t>ld</t>
   </si>
@@ -340,9 +340,6 @@
     <t>-- store Y  to 0x8001</t>
   </si>
   <si>
-    <t>-- store X to 0x8002</t>
-  </si>
-  <si>
     <t>Zero Page Registers</t>
   </si>
   <si>
@@ -377,9 +374,6 @@
   </si>
   <si>
     <t>--load AC</t>
-  </si>
-  <si>
-    <t>-- load X</t>
   </si>
   <si>
     <t>-- load Y</t>
@@ -437,6 +431,12 @@
   </si>
   <si>
     <t>-- branch to BOOT_VECTOR if equal</t>
+  </si>
+  <si>
+    <t>nop</t>
+  </si>
+  <si>
+    <t>-- Set X to 0x55</t>
   </si>
 </sst>
 </file>
@@ -757,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,10 +799,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -828,10 +828,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O3">
         <v>32</v>
@@ -860,10 +860,10 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O4">
         <v>46</v>
@@ -892,10 +892,10 @@
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="O5">
         <v>52</v>
@@ -924,7 +924,7 @@
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -947,7 +947,7 @@
         <v>4</v>
       </c>
       <c r="L7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -1028,7 +1028,7 @@
         <v>232</v>
       </c>
       <c r="E13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F13">
         <v>16</v>
@@ -1058,7 +1058,7 @@
         <v>240</v>
       </c>
       <c r="E15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F15">
         <v>24</v>
@@ -1073,7 +1073,7 @@
         <v>244</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1088,7 +1088,7 @@
         <v>248</v>
       </c>
       <c r="E17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -1103,7 +1103,7 @@
         <v>252</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F18">
         <v>8</v>
@@ -1118,15 +1118,21 @@
         <v>227</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F19">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
       <c r="E20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F20">
         <v>28</v>
@@ -1163,7 +1169,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D23" t="s">
         <v>19</v>
@@ -1172,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:G58" si="1">_xlfn.XLOOKUP(B23,$B$3:$B$19,$C$3:$C$19)</f>
+        <f>_xlfn.XLOOKUP(B23,$B$3:$B$20,$C$3:$C$20)</f>
         <v>192</v>
       </c>
       <c r="H23">
@@ -1180,11 +1186,11 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" ref="I23:I58" si="2">_xlfn.XLOOKUP(D23,$H$3:$H$7,$I$3:$I$7)</f>
+        <f t="shared" ref="I23:I58" si="1">_xlfn.XLOOKUP(D23,$H$3:$H$7,$I$3:$I$7)</f>
         <v>2</v>
       </c>
       <c r="J23">
-        <f t="shared" ref="J23:J59" si="3">G23+H23+I23</f>
+        <f t="shared" ref="J23:J59" si="2">G23+H23+I23</f>
         <v>194</v>
       </c>
       <c r="L23" s="1" t="s">
@@ -1212,28 +1218,28 @@
         <v>28</v>
       </c>
       <c r="S23" t="str">
-        <f t="shared" ref="S23:S60" si="4">DEC2HEX(E23,2)</f>
+        <f t="shared" ref="S23:S60" si="3">DEC2HEX(E23,2)</f>
         <v>00</v>
       </c>
       <c r="T23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="U23" t="str">
-        <f t="shared" ref="U23:U58" si="5">B23</f>
+        <f t="shared" ref="U23:U58" si="4">B23</f>
         <v>st</v>
       </c>
       <c r="V23" s="1" t="s">
         <v>34</v>
       </c>
       <c r="W23" t="str">
-        <f t="shared" ref="W23:W58" si="6">C23</f>
+        <f t="shared" ref="W23:W58" si="5">C23</f>
         <v>[80,D]</v>
       </c>
       <c r="X23" s="1" t="s">
         <v>34</v>
       </c>
       <c r="Y23" t="str">
-        <f t="shared" ref="Y23:Y58" si="7">D23</f>
+        <f t="shared" ref="Y23:Y58" si="6">D23</f>
         <v>AC</v>
       </c>
       <c r="Z23" s="1" t="s">
@@ -1252,7 +1258,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
         <v>21</v>
@@ -1261,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G24:G72" si="7">_xlfn.XLOOKUP(B24,$B$3:$B$20,$C$3:$C$20)</f>
         <v>192</v>
       </c>
       <c r="H24">
@@ -1269,11 +1275,11 @@
         <v>0</v>
       </c>
       <c r="I24">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="3"/>
         <v>195</v>
       </c>
       <c r="L24" s="1" t="str">
@@ -1305,7 +1311,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="T24" s="1" t="str">
@@ -1313,7 +1319,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U24" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>st</v>
       </c>
       <c r="V24" s="1" t="str">
@@ -1321,7 +1327,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W24" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>[80,D]</v>
       </c>
       <c r="X24" s="1" t="str">
@@ -1329,7 +1335,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y24" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>Y</v>
       </c>
       <c r="Z24" s="1" t="s">
@@ -1345,29 +1351,29 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
       </c>
       <c r="E25">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H25">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L25" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1383,7 +1389,7 @@
       </c>
       <c r="O25" t="str">
         <f t="shared" si="12"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="P25" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1398,15 +1404,15 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S25" t="str">
-        <f t="shared" si="4"/>
-        <v>3F</v>
+        <f t="shared" si="3"/>
+        <v>38</v>
       </c>
       <c r="T25" s="1" t="str">
         <f t="shared" si="16"/>
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>ld</v>
       </c>
       <c r="V25" s="1" t="str">
@@ -1414,16 +1420,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W25" t="str">
-        <f t="shared" si="6"/>
-        <v>Y</v>
+        <f t="shared" si="5"/>
+        <v>X</v>
       </c>
       <c r="X25" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y25" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>D</v>
+      </c>
+      <c r="Z25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
@@ -1432,29 +1444,23 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="H26">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J26">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="3"/>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="L26" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1470,7 +1476,7 @@
       </c>
       <c r="O26" t="str">
         <f t="shared" si="12"/>
-        <v>0D</v>
+        <v>02</v>
       </c>
       <c r="P26" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1485,7 +1491,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T26" s="1" t="str">
@@ -1493,28 +1499,26 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U26" t="str">
-        <f t="shared" si="5"/>
-        <v>ld</v>
+        <f t="shared" si="4"/>
+        <v>nop</v>
       </c>
       <c r="V26" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W26" t="str">
-        <f t="shared" si="6"/>
-        <v>[Y,X],AC</v>
+      <c r="W26">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="X26" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y26" t="str">
-        <f t="shared" si="7"/>
-        <v>MEM</v>
-      </c>
-      <c r="Z26" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="Y26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1522,32 +1526,23 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="7"/>
         <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>122</v>
-      </c>
-      <c r="D27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="1"/>
-        <v>192</v>
       </c>
       <c r="H27">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="2"/>
         <v>2</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="3"/>
-        <v>194</v>
       </c>
       <c r="L27" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1563,7 +1558,7 @@
       </c>
       <c r="O27" t="str">
         <f t="shared" si="12"/>
-        <v>C2</v>
+        <v>02</v>
       </c>
       <c r="P27" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1578,36 +1573,34 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S27" t="str">
-        <f t="shared" si="4"/>
-        <v>02</v>
+        <f t="shared" si="3"/>
+        <v>00</v>
       </c>
       <c r="T27" s="1" t="str">
         <f t="shared" si="16"/>
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U27" t="str">
-        <f t="shared" si="5"/>
-        <v>st</v>
+        <f t="shared" si="4"/>
+        <v>nop</v>
       </c>
       <c r="V27" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W27" t="str">
-        <f t="shared" si="6"/>
-        <v>[80,D]</v>
+      <c r="W27">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="X27" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y27" t="str">
-        <f t="shared" si="7"/>
-        <v>AC</v>
-      </c>
-      <c r="Z27" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="Y27">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1615,32 +1608,23 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="H28">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J28">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="L28" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1656,7 +1640,7 @@
       </c>
       <c r="O28" t="str">
         <f t="shared" si="12"/>
-        <v>14</v>
+        <v>02</v>
       </c>
       <c r="P28" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1671,38 +1655,32 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S28" t="str">
-        <f t="shared" si="4"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>00</v>
       </c>
       <c r="T28" s="1" t="str">
         <f t="shared" si="16"/>
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U28" t="str">
-        <f t="shared" si="5"/>
-        <v>ld</v>
+        <f t="shared" si="4"/>
+        <v>nop</v>
       </c>
       <c r="V28" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W28" t="str">
-        <f t="shared" si="6"/>
-        <v>Y</v>
+      <c r="W28">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="X28" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y28" t="str">
-        <f t="shared" si="7"/>
-        <v>D</v>
-      </c>
-      <c r="Z28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD28" s="1" t="s">
-        <v>92</v>
+      <c r="Y28">
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
@@ -1711,32 +1689,23 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="7"/>
         <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>124</v>
-      </c>
-      <c r="D29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29">
-        <v>56</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="1"/>
-        <v>192</v>
       </c>
       <c r="H29">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="3"/>
-        <v>204</v>
+        <v>2</v>
       </c>
       <c r="L29" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1752,7 +1721,7 @@
       </c>
       <c r="O29" t="str">
         <f t="shared" si="12"/>
-        <v>CC</v>
+        <v>02</v>
       </c>
       <c r="P29" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1767,36 +1736,34 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S29" t="str">
-        <f t="shared" si="4"/>
-        <v>38</v>
+        <f t="shared" si="3"/>
+        <v>00</v>
       </c>
       <c r="T29" s="1" t="str">
         <f t="shared" si="16"/>
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U29" t="str">
-        <f t="shared" si="5"/>
-        <v>st</v>
+        <f t="shared" si="4"/>
+        <v>nop</v>
       </c>
       <c r="V29" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W29" t="str">
-        <f t="shared" si="6"/>
-        <v>[Y,X]</v>
+      <c r="W29">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="X29" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y29" t="str">
-        <f t="shared" si="7"/>
-        <v>D</v>
-      </c>
-      <c r="Z29" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="Y29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1807,7 +1774,7 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
@@ -1816,7 +1783,7 @@
         <v>3</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H30">
@@ -1824,11 +1791,11 @@
         <v>0</v>
       </c>
       <c r="I30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L30" s="1" t="str">
@@ -1860,7 +1827,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>03</v>
       </c>
       <c r="T30" s="1" t="str">
@@ -1868,7 +1835,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U30" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>ld</v>
       </c>
       <c r="V30" s="1" t="str">
@@ -1876,7 +1843,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>[80,D]</v>
       </c>
       <c r="X30" s="1" t="str">
@@ -1884,11 +1851,11 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y30" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>MEM</v>
       </c>
       <c r="Z30" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AD30" s="1" t="s">
         <v>93</v>
@@ -1912,7 +1879,7 @@
         <v>55</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>96</v>
       </c>
       <c r="H31">
@@ -1920,11 +1887,11 @@
         <v>0</v>
       </c>
       <c r="I31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="L31" s="1" t="str">
@@ -1956,7 +1923,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="T31" s="1" t="str">
@@ -1964,7 +1931,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U31" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>xor</v>
       </c>
       <c r="V31" s="1" t="str">
@@ -1972,7 +1939,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W31" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>AC</v>
       </c>
       <c r="X31" s="1" t="str">
@@ -1980,11 +1947,11 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y31" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="Z31" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
@@ -2002,7 +1969,7 @@
         <v>32</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="H32">
@@ -2010,11 +1977,11 @@
         <v>0</v>
       </c>
       <c r="I32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J32">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="3"/>
         <v>240</v>
       </c>
       <c r="L32" s="1" t="str">
@@ -2046,7 +2013,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="T32" s="1" t="str">
@@ -2054,7 +2021,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U32" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>beq</v>
       </c>
       <c r="V32" s="1" t="str">
@@ -2062,7 +2029,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X32" s="1" t="str">
@@ -2070,11 +2037,11 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y32" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="Z32" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
@@ -2086,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D33" t="s">
         <v>20</v>
@@ -2095,7 +2062,7 @@
         <v>3</v>
       </c>
       <c r="G33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H33">
@@ -2103,11 +2070,11 @@
         <v>0</v>
       </c>
       <c r="I33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J33">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L33" s="1" t="str">
@@ -2139,7 +2106,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>03</v>
       </c>
       <c r="T33" s="1" t="str">
@@ -2147,7 +2114,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U33" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>ld</v>
       </c>
       <c r="V33" s="1" t="str">
@@ -2155,7 +2122,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W33" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>[80,D]</v>
       </c>
       <c r="X33" s="1" t="str">
@@ -2163,11 +2130,11 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y33" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>MEM</v>
       </c>
       <c r="Z33" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
@@ -2188,7 +2155,7 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>96</v>
       </c>
       <c r="H34">
@@ -2196,11 +2163,11 @@
         <v>0</v>
       </c>
       <c r="I34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J34">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="L34" s="1" t="str">
@@ -2232,7 +2199,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="T34" s="1" t="str">
@@ -2240,7 +2207,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U34" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>xor</v>
       </c>
       <c r="V34" s="1" t="str">
@@ -2248,7 +2215,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W34" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>AC</v>
       </c>
       <c r="X34" s="1" t="str">
@@ -2256,11 +2223,11 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="Z34" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD34" s="1" t="s">
         <v>94</v>
@@ -2281,7 +2248,7 @@
         <v>46</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>240</v>
       </c>
       <c r="H35">
@@ -2289,11 +2256,11 @@
         <v>0</v>
       </c>
       <c r="I35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J35">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="3"/>
         <v>240</v>
       </c>
       <c r="L35" s="1" t="str">
@@ -2325,7 +2292,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2E</v>
       </c>
       <c r="T35" s="1" t="str">
@@ -2333,7 +2300,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>beq</v>
       </c>
       <c r="V35" s="1" t="str">
@@ -2341,7 +2308,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X35" s="1" t="str">
@@ -2349,11 +2316,11 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y35" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="Z35" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
@@ -2374,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="G36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H36">
@@ -2382,11 +2349,11 @@
         <v>0</v>
       </c>
       <c r="I36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J36">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L36" s="1" t="str">
@@ -2418,7 +2385,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S36" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="T36" s="1" t="str">
@@ -2426,7 +2393,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U36" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>ld</v>
       </c>
       <c r="V36" s="1" t="str">
@@ -2434,7 +2401,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W36" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>AC</v>
       </c>
       <c r="X36" s="1" t="str">
@@ -2442,7 +2409,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y36" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="AD36" s="1" t="s">
@@ -2458,7 +2425,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D37" t="s">
         <v>19</v>
@@ -2467,7 +2434,7 @@
         <v>3</v>
       </c>
       <c r="G37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>192</v>
       </c>
       <c r="H37">
@@ -2475,11 +2442,11 @@
         <v>0</v>
       </c>
       <c r="I37">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J37">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="3"/>
         <v>194</v>
       </c>
       <c r="L37" s="1" t="str">
@@ -2511,7 +2478,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S37" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>03</v>
       </c>
       <c r="T37" s="1" t="str">
@@ -2519,7 +2486,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>st</v>
       </c>
       <c r="V37" s="1" t="str">
@@ -2527,7 +2494,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W37" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>[80,D]</v>
       </c>
       <c r="X37" s="1" t="str">
@@ -2535,7 +2502,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y37" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>AC</v>
       </c>
       <c r="Z37" s="1" t="s">
@@ -2551,7 +2518,7 @@
         <v>63</v>
       </c>
       <c r="G38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>227</v>
       </c>
       <c r="H38">
@@ -2559,11 +2526,11 @@
         <v>0</v>
       </c>
       <c r="I38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J38">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="3"/>
         <v>227</v>
       </c>
       <c r="L38" s="1" t="str">
@@ -2595,7 +2562,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S38" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T38" s="1" t="str">
@@ -2603,7 +2570,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>reti</v>
       </c>
       <c r="V38" s="1" t="str">
@@ -2611,7 +2578,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X38" s="1" t="str">
@@ -2619,7 +2586,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Z38" s="1" t="s">
@@ -2647,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <f>_xlfn.XLOOKUP(B39,$B$3:$B$19,$C$3:$C$19)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H39">
@@ -2659,7 +2626,7 @@
         <v>0</v>
       </c>
       <c r="J39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L39" s="1" t="str">
@@ -2722,7 +2689,7 @@
         <v>42</v>
       </c>
       <c r="AD39" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
@@ -2731,32 +2698,23 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="G40">
-        <f>_xlfn.XLOOKUP(B40,$B$3:$B$19,$C$3:$C$19)</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="H40">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I40">
         <f>_xlfn.XLOOKUP(D40,$H$3:$H$7,$I$3:$I$7)</f>
         <v>0</v>
       </c>
       <c r="J40">
-        <f t="shared" si="3"/>
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="L40" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2772,7 +2730,7 @@
       </c>
       <c r="O40" t="str">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>02</v>
       </c>
       <c r="P40" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2796,30 +2754,25 @@
       </c>
       <c r="U40" t="str">
         <f>B40</f>
-        <v>ld</v>
+        <v>nop</v>
       </c>
       <c r="V40" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W40" t="str">
+      <c r="W40">
         <f>C40</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="X40" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y40" t="str">
+      <c r="Y40">
         <f>D40</f>
-        <v>D</v>
-      </c>
-      <c r="Z40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD40" s="1" t="s">
-        <v>97</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -2839,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <f>_xlfn.XLOOKUP(B41,$B$3:$B$19,$C$3:$C$19)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H41">
@@ -2851,7 +2804,7 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="L41" s="1" t="str">
@@ -2929,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H42">
@@ -2937,11 +2890,11 @@
         <v>0</v>
       </c>
       <c r="I42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J42">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L42" s="1" t="str">
@@ -2973,7 +2926,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S42" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T42" s="1" t="str">
@@ -2981,7 +2934,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>ld</v>
       </c>
       <c r="V42" s="1" t="str">
@@ -2989,7 +2942,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W42" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>[80,D],AC</v>
       </c>
       <c r="X42" s="1" t="str">
@@ -2997,11 +2950,14 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y42" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>MEM</v>
       </c>
       <c r="Z42" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="AD42" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.25">
@@ -3010,32 +2966,23 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="G43">
-        <f>_xlfn.XLOOKUP(B43,$B$3:$B$19,$C$3:$C$19)</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="H43">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I43">
         <f>_xlfn.XLOOKUP(D43,$H$3:$H$7,$I$3:$I$7)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="L43" s="1" t="str">
         <f t="shared" si="9"/>
@@ -3051,7 +2998,7 @@
       </c>
       <c r="O43" t="str">
         <f t="shared" si="12"/>
-        <v>11</v>
+        <v>02</v>
       </c>
       <c r="P43" s="1" t="str">
         <f t="shared" si="13"/>
@@ -3067,7 +3014,7 @@
       </c>
       <c r="S43" t="str">
         <f>DEC2HEX(E43,2)</f>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="T43" s="1" t="str">
         <f t="shared" si="16"/>
@@ -3075,27 +3022,25 @@
       </c>
       <c r="U43" t="str">
         <f>B43</f>
-        <v>ld</v>
+        <v>nop</v>
       </c>
       <c r="V43" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W43" t="str">
+      <c r="W43">
         <f>C43</f>
-        <v>[80,D],X</v>
+        <v>0</v>
       </c>
       <c r="X43" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y43" t="str">
+      <c r="Y43">
         <f>D43</f>
-        <v>MEM</v>
-      </c>
-      <c r="Z43" s="1" t="s">
-        <v>113</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -3115,7 +3060,7 @@
         <v>2</v>
       </c>
       <c r="G44">
-        <f>_xlfn.XLOOKUP(B44,$B$3:$B$19,$C$3:$C$19)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H44">
@@ -3127,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="J44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="L44" s="1" t="str">
@@ -3187,7 +3132,7 @@
         <v>MEM</v>
       </c>
       <c r="Z44" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
@@ -3199,7 +3144,7 @@
         <v>63</v>
       </c>
       <c r="G45">
-        <f>_xlfn.XLOOKUP(B45,$B$3:$B$19,$C$3:$C$19)</f>
+        <f t="shared" si="7"/>
         <v>227</v>
       </c>
       <c r="H45">
@@ -3211,7 +3156,7 @@
         <v>0</v>
       </c>
       <c r="J45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>227</v>
       </c>
       <c r="L45" s="1" t="str">
@@ -3292,7 +3237,7 @@
         <v>55</v>
       </c>
       <c r="G46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H46">
@@ -3300,11 +3245,11 @@
         <v>0</v>
       </c>
       <c r="I46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J46">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L46" s="1" t="str">
@@ -3336,7 +3281,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S46" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="T46" s="1" t="str">
@@ -3344,7 +3289,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>ld</v>
       </c>
       <c r="V46" s="1" t="str">
@@ -3352,7 +3297,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>AC</v>
       </c>
       <c r="X46" s="1" t="str">
@@ -3360,12 +3305,12 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y46" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="Z46" s="1"/>
       <c r="AD46" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
@@ -3377,7 +3322,7 @@
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
@@ -3386,7 +3331,7 @@
         <v>3</v>
       </c>
       <c r="G47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>192</v>
       </c>
       <c r="H47">
@@ -3394,11 +3339,11 @@
         <v>0</v>
       </c>
       <c r="I47">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J47">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="3"/>
         <v>194</v>
       </c>
       <c r="L47" s="1" t="str">
@@ -3430,7 +3375,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S47" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>03</v>
       </c>
       <c r="T47" s="1" t="str">
@@ -3438,7 +3383,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>st</v>
       </c>
       <c r="V47" s="1" t="str">
@@ -3446,7 +3391,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>[80,D]</v>
       </c>
       <c r="X47" s="1" t="str">
@@ -3454,11 +3399,11 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y47" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>AC</v>
       </c>
       <c r="Z47" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.25">
@@ -3479,7 +3424,7 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H48">
@@ -3487,11 +3432,11 @@
         <v>0</v>
       </c>
       <c r="I48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J48">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J48">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L48" s="1" t="str">
@@ -3523,7 +3468,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S48" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T48" s="1" t="str">
@@ -3531,7 +3476,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>ld</v>
       </c>
       <c r="V48" s="1" t="str">
@@ -3539,7 +3484,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W48" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>AC</v>
       </c>
       <c r="X48" s="1" t="str">
@@ -3547,14 +3492,14 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y48" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="Z48" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AD48" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
@@ -3566,7 +3511,7 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D49" t="s">
         <v>19</v>
@@ -3575,7 +3520,7 @@
         <v>4</v>
       </c>
       <c r="G49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>192</v>
       </c>
       <c r="H49">
@@ -3583,11 +3528,11 @@
         <v>0</v>
       </c>
       <c r="I49">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J49">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="3"/>
         <v>194</v>
       </c>
       <c r="L49" s="1" t="str">
@@ -3619,7 +3564,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S49" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>04</v>
       </c>
       <c r="T49" s="1" t="str">
@@ -3627,7 +3572,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>st</v>
       </c>
       <c r="V49" s="1" t="str">
@@ -3635,7 +3580,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W49" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>[80,D]</v>
       </c>
       <c r="X49" s="1" t="str">
@@ -3643,14 +3588,14 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y49" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>AC</v>
       </c>
       <c r="Z49" s="1" t="s">
         <v>82</v>
       </c>
       <c r="AD49" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.25">
@@ -3662,7 +3607,7 @@
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D50" t="s">
         <v>20</v>
@@ -3671,7 +3616,7 @@
         <v>4</v>
       </c>
       <c r="G50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H50">
@@ -3679,11 +3624,11 @@
         <v>0</v>
       </c>
       <c r="I50">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J50">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J50">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L50" s="1" t="str">
@@ -3715,7 +3660,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S50" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>04</v>
       </c>
       <c r="T50" s="1" t="str">
@@ -3723,7 +3668,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>ld</v>
       </c>
       <c r="V50" s="1" t="str">
@@ -3731,7 +3676,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W50" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>[80,D]</v>
       </c>
       <c r="X50" s="1" t="str">
@@ -3739,7 +3684,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y50" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>MEM</v>
       </c>
       <c r="Z50" s="1" t="s">
@@ -3764,7 +3709,7 @@
         <v>1</v>
       </c>
       <c r="G51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>128</v>
       </c>
       <c r="H51">
@@ -3772,11 +3717,11 @@
         <v>0</v>
       </c>
       <c r="I51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J51">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J51">
-        <f t="shared" si="3"/>
         <v>128</v>
       </c>
       <c r="L51" s="1" t="str">
@@ -3808,7 +3753,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S51" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>01</v>
       </c>
       <c r="T51" s="1" t="str">
@@ -3816,7 +3761,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>add</v>
       </c>
       <c r="V51" s="1" t="str">
@@ -3824,7 +3769,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W51" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>AC</v>
       </c>
       <c r="X51" s="1" t="str">
@@ -3832,7 +3777,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y51" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="Z51" s="1" t="s">
@@ -3848,13 +3793,13 @@
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D52" t="s">
         <v>19</v>
       </c>
       <c r="G52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H52">
@@ -3862,11 +3807,11 @@
         <v>24</v>
       </c>
       <c r="I52">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J52">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J52">
-        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="L52" s="1" t="str">
@@ -3898,7 +3843,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S52" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T52" s="1" t="str">
@@ -3906,7 +3851,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>ld</v>
       </c>
       <c r="V52" s="1" t="str">
@@ -3914,7 +3859,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W52" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>VID</v>
       </c>
       <c r="X52" s="1" t="str">
@@ -3922,11 +3867,11 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y52" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>AC</v>
       </c>
       <c r="Z52" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
@@ -3944,7 +3889,7 @@
         <v>52</v>
       </c>
       <c r="G53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>252</v>
       </c>
       <c r="H53">
@@ -3952,11 +3897,11 @@
         <v>0</v>
       </c>
       <c r="I53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J53">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J53">
-        <f t="shared" si="3"/>
         <v>252</v>
       </c>
       <c r="L53" s="1" t="str">
@@ -3988,7 +3933,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S53" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="T53" s="1" t="str">
@@ -3996,7 +3941,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>bra</v>
       </c>
       <c r="V53" s="1" t="str">
@@ -4004,7 +3949,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X53" s="1" t="str">
@@ -4012,11 +3957,11 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y53" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>D</v>
       </c>
       <c r="Z53" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.25">
@@ -4025,7 +3970,7 @@
         <v>62</v>
       </c>
       <c r="G54" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H54">
@@ -4033,11 +3978,11 @@
         <v>0</v>
       </c>
       <c r="I54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J54" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J54" t="e">
-        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="L54" s="1" t="str">
@@ -4069,7 +4014,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S54" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T54" s="1" t="str">
@@ -4077,7 +4022,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V54" s="1" t="str">
@@ -4085,7 +4030,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X54" s="1" t="str">
@@ -4093,7 +4038,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4103,7 +4048,7 @@
         <v>64</v>
       </c>
       <c r="G55" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H55">
@@ -4111,11 +4056,11 @@
         <v>0</v>
       </c>
       <c r="I55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J55" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J55" t="e">
-        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="L55" s="1" t="str">
@@ -4147,7 +4092,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S55" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T55" s="1" t="str">
@@ -4155,7 +4100,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V55" s="1" t="str">
@@ -4163,7 +4108,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X55" s="1" t="str">
@@ -4171,7 +4116,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4181,7 +4126,7 @@
         <v>66</v>
       </c>
       <c r="G56" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H56">
@@ -4189,11 +4134,11 @@
         <v>0</v>
       </c>
       <c r="I56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J56" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J56" t="e">
-        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="L56" s="1" t="str">
@@ -4225,7 +4170,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S56" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T56" s="1" t="str">
@@ -4233,7 +4178,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V56" s="1" t="str">
@@ -4241,7 +4186,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X56" s="1" t="str">
@@ -4249,7 +4194,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Z56" s="1"/>
@@ -4260,7 +4205,7 @@
         <v>68</v>
       </c>
       <c r="G57" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H57">
@@ -4268,11 +4213,11 @@
         <v>0</v>
       </c>
       <c r="I57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J57" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J57" t="e">
-        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="L57" s="1" t="str">
@@ -4304,7 +4249,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S57" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T57" s="1" t="str">
@@ -4312,7 +4257,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V57" s="1" t="str">
@@ -4320,7 +4265,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X57" s="1" t="str">
@@ -4328,7 +4273,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4338,7 +4283,7 @@
         <v>70</v>
       </c>
       <c r="G58" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H58">
@@ -4346,11 +4291,11 @@
         <v>0</v>
       </c>
       <c r="I58">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J58" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J58" t="e">
-        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="L58" s="1" t="str">
@@ -4382,7 +4327,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S58" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T58" s="1" t="str">
@@ -4390,7 +4335,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="V58" s="1" t="str">
@@ -4398,7 +4343,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X58" s="1" t="str">
@@ -4406,7 +4351,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4416,7 +4361,7 @@
         <v>72</v>
       </c>
       <c r="G59" t="e">
-        <f>_xlfn.XLOOKUP(B59,$B$3:$B$19,$C$3:$C$19)</f>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H59">
@@ -4428,7 +4373,7 @@
         <v>0</v>
       </c>
       <c r="J59" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="L59" s="1" t="str">
@@ -4460,7 +4405,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S59" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T59" s="1" t="str">
@@ -4495,7 +4440,7 @@
         <v>74</v>
       </c>
       <c r="G60" t="e">
-        <f>_xlfn.XLOOKUP(B60,$B$3:$B$19,$C$3:$C$19)</f>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H60">
@@ -4539,7 +4484,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S60" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>00</v>
       </c>
       <c r="T60" s="1" t="str">
@@ -4573,7 +4518,7 @@
         <v>76</v>
       </c>
       <c r="G61" t="e">
-        <f>_xlfn.XLOOKUP(B61,$B$3:$B$19,$C$3:$C$19)</f>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H61">
@@ -4652,7 +4597,7 @@
         <v>78</v>
       </c>
       <c r="G62" t="e">
-        <f>_xlfn.XLOOKUP(B62,$B$3:$B$19,$C$3:$C$19)</f>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H62">
@@ -4731,7 +4676,7 @@
         <v>80</v>
       </c>
       <c r="G63" t="e">
-        <f t="shared" ref="G63:G65" si="28">_xlfn.XLOOKUP(B63,$B$3:$B$19,$C$3:$C$19)</f>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H63">
@@ -4739,7 +4684,7 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <f t="shared" ref="I63:I65" si="29">_xlfn.XLOOKUP(D63,$H$3:$H$7,$I$3:$I$7)</f>
+        <f t="shared" ref="I63:I65" si="28">_xlfn.XLOOKUP(D63,$H$3:$H$7,$I$3:$I$7)</f>
         <v>0</v>
       </c>
       <c r="J63" t="e">
@@ -4783,7 +4728,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U63">
-        <f t="shared" ref="U63:U65" si="30">B63</f>
+        <f t="shared" ref="U63:U65" si="29">B63</f>
         <v>0</v>
       </c>
       <c r="V63" s="1" t="str">
@@ -4791,7 +4736,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W63">
-        <f t="shared" ref="W63:W65" si="31">C63</f>
+        <f t="shared" ref="W63:W65" si="30">C63</f>
         <v>0</v>
       </c>
       <c r="X63" s="1" t="str">
@@ -4799,7 +4744,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y63">
-        <f t="shared" ref="Y63:Y65" si="32">D63</f>
+        <f t="shared" ref="Y63:Y65" si="31">D63</f>
         <v>0</v>
       </c>
       <c r="Z63" s="1"/>
@@ -4810,7 +4755,7 @@
         <v>82</v>
       </c>
       <c r="G64" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H64">
@@ -4818,7 +4763,7 @@
         <v>0</v>
       </c>
       <c r="I64">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="J64" t="e">
@@ -4862,7 +4807,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U64">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="V64" s="1" t="str">
@@ -4870,7 +4815,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W64">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="X64" s="1" t="str">
@@ -4878,7 +4823,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y64">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
@@ -4888,7 +4833,7 @@
         <v>84</v>
       </c>
       <c r="G65" t="e">
-        <f t="shared" si="28"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H65">
@@ -4896,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="I65">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="J65" t="e">
@@ -4940,7 +4885,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U65">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="V65" s="1" t="str">
@@ -4948,7 +4893,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W65">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="X65" s="1" t="str">
@@ -4956,7 +4901,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y65">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="Z65" s="1"/>
@@ -4967,7 +4912,7 @@
         <v>86</v>
       </c>
       <c r="G66" t="e">
-        <f t="shared" ref="G66:G72" si="33">_xlfn.XLOOKUP(B66,$B$3:$B$19,$C$3:$C$19)</f>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="H66">
@@ -4975,11 +4920,11 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <f t="shared" ref="I66:I72" si="34">_xlfn.XLOOKUP(D66,$H$3:$H$7,$I$3:$I$7)</f>
+        <f t="shared" ref="I66:I72" si="32">_xlfn.XLOOKUP(D66,$H$3:$H$7,$I$3:$I$7)</f>
         <v>0</v>
       </c>
       <c r="J66" t="e">
-        <f t="shared" ref="J66:J72" si="35">G66+H66+I66</f>
+        <f t="shared" ref="J66:J72" si="33">G66+H66+I66</f>
         <v>#N/A</v>
       </c>
       <c r="L66" s="1" t="str">
@@ -4987,7 +4932,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="M66">
-        <f t="shared" ref="M66:M72" si="36">A66</f>
+        <f t="shared" ref="M66:M72" si="34">A66</f>
         <v>86</v>
       </c>
       <c r="N66" s="1" t="str">
@@ -4995,7 +4940,7 @@
         <v xml:space="preserve"> =&gt;x"</v>
       </c>
       <c r="O66" t="e">
-        <f t="shared" ref="O66:O72" si="37">DEC2HEX(J66,2)</f>
+        <f t="shared" ref="O66:O72" si="35">DEC2HEX(J66,2)</f>
         <v>#N/A</v>
       </c>
       <c r="P66" s="1" t="str">
@@ -5003,7 +4948,7 @@
         <v xml:space="preserve">",  </v>
       </c>
       <c r="Q66">
-        <f t="shared" ref="Q66:Q72" si="38">M66+1</f>
+        <f t="shared" ref="Q66:Q72" si="36">M66+1</f>
         <v>87</v>
       </c>
       <c r="R66" s="1" t="str">
@@ -5011,7 +4956,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S66" t="str">
-        <f t="shared" ref="S66:S72" si="39">DEC2HEX(E66,2)</f>
+        <f t="shared" ref="S66:S72" si="37">DEC2HEX(E66,2)</f>
         <v>00</v>
       </c>
       <c r="T66" s="1" t="str">
@@ -5019,7 +4964,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U66">
-        <f t="shared" ref="U66:U72" si="40">B66</f>
+        <f t="shared" ref="U66:U72" si="38">B66</f>
         <v>0</v>
       </c>
       <c r="V66" s="1" t="str">
@@ -5027,7 +4972,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W66">
-        <f t="shared" ref="W66:W72" si="41">C66</f>
+        <f t="shared" ref="W66:W72" si="39">C66</f>
         <v>0</v>
       </c>
       <c r="X66" s="1" t="str">
@@ -5035,7 +4980,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y66">
-        <f t="shared" ref="Y66:Y72" si="42">D66</f>
+        <f t="shared" ref="Y66:Y72" si="40">D66</f>
         <v>0</v>
       </c>
     </row>
@@ -5045,27 +4990,27 @@
         <v>88</v>
       </c>
       <c r="G67" t="e">
+        <f t="shared" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J67" t="e">
         <f t="shared" si="33"/>
         <v>#N/A</v>
       </c>
-      <c r="H67">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I67">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="J67" t="e">
-        <f t="shared" si="35"/>
-        <v>#N/A</v>
-      </c>
       <c r="L67" s="1" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M67">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>88</v>
       </c>
       <c r="N67" s="1" t="str">
@@ -5073,7 +5018,7 @@
         <v xml:space="preserve"> =&gt;x"</v>
       </c>
       <c r="O67" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>#N/A</v>
       </c>
       <c r="P67" s="1" t="str">
@@ -5081,7 +5026,7 @@
         <v xml:space="preserve">",  </v>
       </c>
       <c r="Q67">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>89</v>
       </c>
       <c r="R67" s="1" t="str">
@@ -5089,7 +5034,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S67" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>00</v>
       </c>
       <c r="T67" s="1" t="str">
@@ -5097,7 +5042,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U67">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="V67" s="1" t="str">
@@ -5105,7 +5050,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W67">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X67" s="1" t="str">
@@ -5113,7 +5058,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y67">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Z67" s="1"/>
@@ -5124,27 +5069,27 @@
         <v>90</v>
       </c>
       <c r="G68" t="e">
+        <f t="shared" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J68" t="e">
         <f t="shared" si="33"/>
         <v>#N/A</v>
       </c>
-      <c r="H68">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I68">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="J68" t="e">
-        <f t="shared" si="35"/>
-        <v>#N/A</v>
-      </c>
       <c r="L68" s="1" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M68">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>90</v>
       </c>
       <c r="N68" s="1" t="str">
@@ -5152,7 +5097,7 @@
         <v xml:space="preserve"> =&gt;x"</v>
       </c>
       <c r="O68" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>#N/A</v>
       </c>
       <c r="P68" s="1" t="str">
@@ -5160,7 +5105,7 @@
         <v xml:space="preserve">",  </v>
       </c>
       <c r="Q68">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>91</v>
       </c>
       <c r="R68" s="1" t="str">
@@ -5168,7 +5113,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S68" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>00</v>
       </c>
       <c r="T68" s="1" t="str">
@@ -5176,7 +5121,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U68">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="V68" s="1" t="str">
@@ -5184,7 +5129,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W68">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X68" s="1" t="str">
@@ -5192,7 +5137,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y68">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Z68" s="1"/>
@@ -5203,27 +5148,27 @@
         <v>92</v>
       </c>
       <c r="G69" t="e">
+        <f t="shared" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J69" t="e">
         <f t="shared" si="33"/>
         <v>#N/A</v>
       </c>
-      <c r="H69">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I69">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="J69" t="e">
-        <f t="shared" si="35"/>
-        <v>#N/A</v>
-      </c>
       <c r="L69" s="1" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M69">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>92</v>
       </c>
       <c r="N69" s="1" t="str">
@@ -5231,7 +5176,7 @@
         <v xml:space="preserve"> =&gt;x"</v>
       </c>
       <c r="O69" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>#N/A</v>
       </c>
       <c r="P69" s="1" t="str">
@@ -5239,7 +5184,7 @@
         <v xml:space="preserve">",  </v>
       </c>
       <c r="Q69">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>93</v>
       </c>
       <c r="R69" s="1" t="str">
@@ -5247,7 +5192,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S69" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>00</v>
       </c>
       <c r="T69" s="1" t="str">
@@ -5255,7 +5200,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U69">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="V69" s="1" t="str">
@@ -5263,7 +5208,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W69">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X69" s="1" t="str">
@@ -5271,7 +5216,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y69">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
@@ -5281,27 +5226,27 @@
         <v>94</v>
       </c>
       <c r="G70" t="e">
+        <f t="shared" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J70" t="e">
         <f t="shared" si="33"/>
         <v>#N/A</v>
       </c>
-      <c r="H70">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="J70" t="e">
-        <f t="shared" si="35"/>
-        <v>#N/A</v>
-      </c>
       <c r="L70" s="1" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M70">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>94</v>
       </c>
       <c r="N70" s="1" t="str">
@@ -5309,7 +5254,7 @@
         <v xml:space="preserve"> =&gt;x"</v>
       </c>
       <c r="O70" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>#N/A</v>
       </c>
       <c r="P70" s="1" t="str">
@@ -5317,7 +5262,7 @@
         <v xml:space="preserve">",  </v>
       </c>
       <c r="Q70">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>95</v>
       </c>
       <c r="R70" s="1" t="str">
@@ -5325,7 +5270,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S70" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>00</v>
       </c>
       <c r="T70" s="1" t="str">
@@ -5333,7 +5278,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U70">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="V70" s="1" t="str">
@@ -5341,7 +5286,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W70">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X70" s="1" t="str">
@@ -5349,7 +5294,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y70">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
@@ -5359,27 +5304,27 @@
         <v>96</v>
       </c>
       <c r="G71" t="e">
+        <f t="shared" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J71" t="e">
         <f t="shared" si="33"/>
         <v>#N/A</v>
       </c>
-      <c r="H71">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I71">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="J71" t="e">
-        <f t="shared" si="35"/>
-        <v>#N/A</v>
-      </c>
       <c r="L71" s="1" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M71">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>96</v>
       </c>
       <c r="N71" s="1" t="str">
@@ -5387,7 +5332,7 @@
         <v xml:space="preserve"> =&gt;x"</v>
       </c>
       <c r="O71" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>#N/A</v>
       </c>
       <c r="P71" s="1" t="str">
@@ -5395,7 +5340,7 @@
         <v xml:space="preserve">",  </v>
       </c>
       <c r="Q71">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>97</v>
       </c>
       <c r="R71" s="1" t="str">
@@ -5403,7 +5348,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S71" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>00</v>
       </c>
       <c r="T71" s="1" t="str">
@@ -5411,7 +5356,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U71">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="V71" s="1" t="str">
@@ -5419,7 +5364,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W71">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X71" s="1" t="str">
@@ -5427,7 +5372,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y71">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
@@ -5437,27 +5382,27 @@
         <v>98</v>
       </c>
       <c r="G72" t="e">
+        <f t="shared" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J72" t="e">
         <f t="shared" si="33"/>
         <v>#N/A</v>
       </c>
-      <c r="H72">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I72">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="J72" t="e">
-        <f t="shared" si="35"/>
-        <v>#N/A</v>
-      </c>
       <c r="L72" s="1" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M72">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>98</v>
       </c>
       <c r="N72" s="1" t="str">
@@ -5465,7 +5410,7 @@
         <v xml:space="preserve"> =&gt;x"</v>
       </c>
       <c r="O72" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>#N/A</v>
       </c>
       <c r="P72" s="1" t="str">
@@ -5473,7 +5418,7 @@
         <v xml:space="preserve">",  </v>
       </c>
       <c r="Q72">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>99</v>
       </c>
       <c r="R72" s="1" t="str">
@@ -5481,7 +5426,7 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S72" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>00</v>
       </c>
       <c r="T72" s="1" t="str">
@@ -5489,7 +5434,7 @@
         <v xml:space="preserve">", -- </v>
       </c>
       <c r="U72">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="V72" s="1" t="str">
@@ -5497,7 +5442,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="W72">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X72" s="1" t="str">
@@ -5505,7 +5450,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y72">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove xBus.  Change assembly to conform with the new architecture.
</commit_message>
<xml_diff>
--- a/resources/Assembly.xlsx
+++ b/resources/Assembly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\gtxl\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12050C4-81AE-4CF3-BED7-73ED8D1B6C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B45A2D1-A803-457B-8BA8-949FE421C09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5505" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67080" yWindow="-5625" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="127">
   <si>
     <t>ld</t>
   </si>
@@ -280,12 +280,6 @@
     <t>--move n+1 to vid for output</t>
   </si>
   <si>
-    <t>--store 0x01 to BOOTCNT</t>
-  </si>
-  <si>
-    <t>-- reti to set interrupt enbale</t>
-  </si>
-  <si>
     <t>--store value</t>
   </si>
   <si>
@@ -322,19 +316,10 @@
     <t>--check if booting finished</t>
   </si>
   <si>
-    <t>--check if first boot</t>
-  </si>
-  <si>
-    <t>--first boot</t>
-  </si>
-  <si>
     <t>-- return from interrupt</t>
   </si>
   <si>
     <t>--restore registers</t>
-  </si>
-  <si>
-    <t>-- reti to clear interrupt disable for normal booting</t>
   </si>
   <si>
     <t>-- store Y  to 0x8001</t>
@@ -365,9 +350,6 @@
   </si>
   <si>
     <t>VIDEO_HANDLER</t>
-  </si>
-  <si>
-    <t>-- xor compare with 1</t>
   </si>
   <si>
     <t>BOOT_VECTOR</t>
@@ -415,9 +397,6 @@
     <t>[80,X]</t>
   </si>
   <si>
-    <t>--branch if equal to VIDEO_HANDLER</t>
-  </si>
-  <si>
     <t>-- VIDEO_HANDLER</t>
   </si>
   <si>
@@ -430,13 +409,16 @@
     <t>-- branch back to MAIN_LOOP</t>
   </si>
   <si>
-    <t>-- branch to BOOT_VECTOR if equal</t>
-  </si>
-  <si>
     <t>nop</t>
   </si>
   <si>
     <t>-- Set X to 0x55</t>
+  </si>
+  <si>
+    <t>-- branch to BOOT_VECTOR if not equal</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -757,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23:AD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,10 +781,10 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
@@ -813,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -828,13 +810,13 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="M3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="O3">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -860,10 +842,10 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="M4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="O4">
         <v>46</v>
@@ -877,7 +859,7 @@
         <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F5">
         <v>8</v>
@@ -892,10 +874,10 @@
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="M5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="O5">
         <v>52</v>
@@ -924,7 +906,7 @@
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -935,7 +917,7 @@
         <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F7">
         <v>16</v>
@@ -947,7 +929,7 @@
         <v>4</v>
       </c>
       <c r="L7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -958,7 +940,7 @@
         <v>160</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F8">
         <v>20</v>
@@ -972,7 +954,7 @@
         <v>192</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F9">
         <v>24</v>
@@ -1028,7 +1010,7 @@
         <v>232</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F13">
         <v>16</v>
@@ -1058,7 +1040,7 @@
         <v>240</v>
       </c>
       <c r="E15" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F15">
         <v>24</v>
@@ -1073,7 +1055,7 @@
         <v>244</v>
       </c>
       <c r="E16" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1088,7 +1070,7 @@
         <v>248</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -1103,7 +1085,7 @@
         <v>252</v>
       </c>
       <c r="E18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F18">
         <v>8</v>
@@ -1118,7 +1100,7 @@
         <v>227</v>
       </c>
       <c r="E19" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F19">
         <v>12</v>
@@ -1126,13 +1108,13 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F20">
         <v>28</v>
@@ -1169,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D23" t="s">
         <v>19</v>
@@ -1246,7 +1228,7 @@
         <v>38</v>
       </c>
       <c r="AD23" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
@@ -1258,7 +1240,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
         <v>21</v>
@@ -1339,7 +1321,7 @@
         <v>Y</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
@@ -1351,7 +1333,7 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
@@ -1432,10 +1414,10 @@
         <v>D</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="AD25" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
@@ -1444,11 +1426,20 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
       </c>
       <c r="G26">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H26">
         <f t="shared" si="8"/>
@@ -1456,11 +1447,11 @@
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L26" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1476,7 +1467,7 @@
       </c>
       <c r="O26" t="str">
         <f t="shared" si="12"/>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="P26" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1492,7 +1483,7 @@
       </c>
       <c r="S26" t="str">
         <f t="shared" si="3"/>
-        <v>00</v>
+        <v>03</v>
       </c>
       <c r="T26" s="1" t="str">
         <f t="shared" si="16"/>
@@ -1500,25 +1491,30 @@
       </c>
       <c r="U26" t="str">
         <f t="shared" si="4"/>
-        <v>nop</v>
+        <v>ld</v>
       </c>
       <c r="V26" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W26">
+      <c r="W26" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>[80,D]</v>
       </c>
       <c r="X26" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y26">
+      <c r="Y26" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Z26" s="1"/>
+        <v>MEM</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD26" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1526,11 +1522,20 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27">
+        <v>55</v>
       </c>
       <c r="G27">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="H27">
         <f t="shared" si="8"/>
@@ -1542,7 +1547,7 @@
       </c>
       <c r="J27">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="L27" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1558,7 +1563,7 @@
       </c>
       <c r="O27" t="str">
         <f t="shared" si="12"/>
-        <v>02</v>
+        <v>60</v>
       </c>
       <c r="P27" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1574,7 +1579,7 @@
       </c>
       <c r="S27" t="str">
         <f t="shared" si="3"/>
-        <v>00</v>
+        <v>37</v>
       </c>
       <c r="T27" s="1" t="str">
         <f t="shared" si="16"/>
@@ -1582,25 +1587,27 @@
       </c>
       <c r="U27" t="str">
         <f t="shared" si="4"/>
-        <v>nop</v>
+        <v>xor</v>
       </c>
       <c r="V27" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W27">
+      <c r="W27" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>AC</v>
       </c>
       <c r="X27" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y27">
+      <c r="Y27" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Z27" s="1"/>
+        <v>D</v>
+      </c>
+      <c r="Z27" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1608,11 +1615,17 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28">
+        <v>46</v>
       </c>
       <c r="G28">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>236</v>
       </c>
       <c r="H28">
         <f t="shared" si="8"/>
@@ -1624,7 +1637,7 @@
       </c>
       <c r="J28">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>236</v>
       </c>
       <c r="L28" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1640,7 +1653,7 @@
       </c>
       <c r="O28" t="str">
         <f t="shared" si="12"/>
-        <v>02</v>
+        <v>EC</v>
       </c>
       <c r="P28" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1656,7 +1669,7 @@
       </c>
       <c r="S28" t="str">
         <f t="shared" si="3"/>
-        <v>00</v>
+        <v>2E</v>
       </c>
       <c r="T28" s="1" t="str">
         <f t="shared" si="16"/>
@@ -1664,7 +1677,7 @@
       </c>
       <c r="U28" t="str">
         <f t="shared" si="4"/>
-        <v>nop</v>
+        <v>bne</v>
       </c>
       <c r="V28" s="1" t="str">
         <f t="shared" si="17"/>
@@ -1678,9 +1691,12 @@
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y28">
+      <c r="Y28" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>D</v>
+      </c>
+      <c r="Z28" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
@@ -1689,11 +1705,20 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>131</v>
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
       </c>
       <c r="G29">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H29">
         <f t="shared" si="8"/>
@@ -1705,7 +1730,7 @@
       </c>
       <c r="J29">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L29" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1721,7 +1746,7 @@
       </c>
       <c r="O29" t="str">
         <f t="shared" si="12"/>
-        <v>02</v>
+        <v>00</v>
       </c>
       <c r="P29" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1745,25 +1770,30 @@
       </c>
       <c r="U29" t="str">
         <f t="shared" si="4"/>
-        <v>nop</v>
+        <v>ld</v>
       </c>
       <c r="V29" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W29">
+      <c r="W29" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>AC</v>
       </c>
       <c r="X29" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y29">
+      <c r="Y29" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Z29" s="1"/>
+        <v>D</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD29" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1774,13 +1804,13 @@
         <v>0</v>
       </c>
       <c r="C30" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G30">
         <f t="shared" si="7"/>
@@ -1788,15 +1818,15 @@
       </c>
       <c r="H30">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I30">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L30" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1812,7 +1842,7 @@
       </c>
       <c r="O30" t="str">
         <f t="shared" si="12"/>
-        <v>01</v>
+        <v>14</v>
       </c>
       <c r="P30" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1828,7 +1858,7 @@
       </c>
       <c r="S30" t="str">
         <f t="shared" si="3"/>
-        <v>03</v>
+        <v>00</v>
       </c>
       <c r="T30" s="1" t="str">
         <f t="shared" si="16"/>
@@ -1844,7 +1874,7 @@
       </c>
       <c r="W30" t="str">
         <f t="shared" si="5"/>
-        <v>[80,D]</v>
+        <v>y</v>
       </c>
       <c r="X30" s="1" t="str">
         <f t="shared" si="18"/>
@@ -1852,14 +1882,9 @@
       </c>
       <c r="Y30" t="str">
         <f t="shared" si="6"/>
-        <v>MEM</v>
-      </c>
-      <c r="Z30" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD30" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>D</v>
+      </c>
+      <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1867,20 +1892,20 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E31">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <f t="shared" si="7"/>
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="H31">
         <f t="shared" si="8"/>
@@ -1888,11 +1913,11 @@
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31">
         <f t="shared" si="2"/>
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="L31" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1908,7 +1933,7 @@
       </c>
       <c r="O31" t="str">
         <f t="shared" si="12"/>
-        <v>60</v>
+        <v>01</v>
       </c>
       <c r="P31" s="1" t="str">
         <f t="shared" si="13"/>
@@ -1924,7 +1949,7 @@
       </c>
       <c r="S31" t="str">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>00</v>
       </c>
       <c r="T31" s="1" t="str">
         <f t="shared" si="16"/>
@@ -1932,7 +1957,7 @@
       </c>
       <c r="U31" t="str">
         <f t="shared" si="4"/>
-        <v>xor</v>
+        <v>ld</v>
       </c>
       <c r="V31" s="1" t="str">
         <f t="shared" si="17"/>
@@ -1940,7 +1965,7 @@
       </c>
       <c r="W31" t="str">
         <f t="shared" si="5"/>
-        <v>AC</v>
+        <v>[80,D],AC</v>
       </c>
       <c r="X31" s="1" t="str">
         <f t="shared" si="18"/>
@@ -1948,10 +1973,13 @@
       </c>
       <c r="Y31" t="str">
         <f t="shared" si="6"/>
-        <v>D</v>
+        <v>MEM</v>
       </c>
       <c r="Z31" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="AD31" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
@@ -1960,29 +1988,32 @@
         <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
       </c>
       <c r="D32" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E32">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <f t="shared" si="7"/>
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="H32">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32">
         <f t="shared" si="2"/>
-        <v>240</v>
+        <v>21</v>
       </c>
       <c r="L32" s="1" t="str">
         <f t="shared" si="9"/>
@@ -1998,7 +2029,7 @@
       </c>
       <c r="O32" t="str">
         <f t="shared" si="12"/>
-        <v>F0</v>
+        <v>15</v>
       </c>
       <c r="P32" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2013,8 +2044,8 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S32" t="str">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f>DEC2HEX(E32,2)</f>
+        <v>01</v>
       </c>
       <c r="T32" s="1" t="str">
         <f t="shared" si="16"/>
@@ -2022,15 +2053,15 @@
       </c>
       <c r="U32" t="str">
         <f t="shared" si="4"/>
-        <v>beq</v>
+        <v>ld</v>
       </c>
       <c r="V32" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W32">
+      <c r="W32" t="str">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>[80,D],Y</v>
       </c>
       <c r="X32" s="1" t="str">
         <f t="shared" si="18"/>
@@ -2038,10 +2069,10 @@
       </c>
       <c r="Y32" t="str">
         <f t="shared" si="6"/>
-        <v>D</v>
+        <v>MEM</v>
       </c>
       <c r="Z32" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
@@ -2050,20 +2081,11 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="G33">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>227</v>
       </c>
       <c r="H33">
         <f t="shared" si="8"/>
@@ -2071,11 +2093,11 @@
       </c>
       <c r="I33">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>227</v>
       </c>
       <c r="L33" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2091,7 +2113,7 @@
       </c>
       <c r="O33" t="str">
         <f t="shared" si="12"/>
-        <v>01</v>
+        <v>E3</v>
       </c>
       <c r="P33" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2107,7 +2129,7 @@
       </c>
       <c r="S33" t="str">
         <f t="shared" si="3"/>
-        <v>03</v>
+        <v>00</v>
       </c>
       <c r="T33" s="1" t="str">
         <f t="shared" si="16"/>
@@ -2115,26 +2137,26 @@
       </c>
       <c r="U33" t="str">
         <f t="shared" si="4"/>
-        <v>ld</v>
+        <v>reti</v>
       </c>
       <c r="V33" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W33" t="str">
+      <c r="W33">
         <f t="shared" si="5"/>
-        <v>[80,D]</v>
+        <v>0</v>
       </c>
       <c r="X33" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y33" t="str">
+      <c r="Y33">
         <f t="shared" si="6"/>
-        <v>MEM</v>
+        <v>0</v>
       </c>
       <c r="Z33" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
@@ -2143,20 +2165,11 @@
         <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="G34">
         <f t="shared" si="7"/>
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="H34">
         <f t="shared" si="8"/>
@@ -2168,7 +2181,7 @@
       </c>
       <c r="J34">
         <f t="shared" si="2"/>
-        <v>96</v>
+        <v>2</v>
       </c>
       <c r="L34" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2184,7 +2197,7 @@
       </c>
       <c r="O34" t="str">
         <f t="shared" si="12"/>
-        <v>60</v>
+        <v>02</v>
       </c>
       <c r="P34" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2200,7 +2213,7 @@
       </c>
       <c r="S34" t="str">
         <f t="shared" si="3"/>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="T34" s="1" t="str">
         <f t="shared" si="16"/>
@@ -2208,30 +2221,26 @@
       </c>
       <c r="U34" t="str">
         <f t="shared" si="4"/>
-        <v>xor</v>
+        <v>nop</v>
       </c>
       <c r="V34" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W34" t="str">
+      <c r="W34">
         <f t="shared" si="5"/>
-        <v>AC</v>
+        <v>0</v>
       </c>
       <c r="X34" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y34" t="str">
+      <c r="Y34">
         <f t="shared" si="6"/>
-        <v>D</v>
-      </c>
-      <c r="Z34" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD34" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Z34" s="1"/>
+      <c r="AD34" s="1"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -2239,17 +2248,11 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35">
-        <v>46</v>
+        <v>123</v>
       </c>
       <c r="G35">
         <f t="shared" si="7"/>
-        <v>240</v>
+        <v>2</v>
       </c>
       <c r="H35">
         <f t="shared" si="8"/>
@@ -2261,7 +2264,7 @@
       </c>
       <c r="J35">
         <f t="shared" si="2"/>
-        <v>240</v>
+        <v>2</v>
       </c>
       <c r="L35" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2277,7 +2280,7 @@
       </c>
       <c r="O35" t="str">
         <f t="shared" si="12"/>
-        <v>F0</v>
+        <v>02</v>
       </c>
       <c r="P35" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2292,8 +2295,8 @@
         <v>=&gt;x"</v>
       </c>
       <c r="S35" t="str">
-        <f t="shared" si="3"/>
-        <v>2E</v>
+        <f>DEC2HEX(E35,2)</f>
+        <v>00</v>
       </c>
       <c r="T35" s="1" t="str">
         <f t="shared" si="16"/>
@@ -2301,7 +2304,7 @@
       </c>
       <c r="U35" t="str">
         <f t="shared" si="4"/>
-        <v>beq</v>
+        <v>nop</v>
       </c>
       <c r="V35" s="1" t="str">
         <f t="shared" si="17"/>
@@ -2315,12 +2318,9 @@
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y35" t="str">
+      <c r="Y35">
         <f t="shared" si="6"/>
-        <v>D</v>
-      </c>
-      <c r="Z35" s="1" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
@@ -2329,20 +2329,11 @@
         <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="G36">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36">
         <f t="shared" si="8"/>
@@ -2354,7 +2345,7 @@
       </c>
       <c r="J36">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L36" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2370,7 +2361,7 @@
       </c>
       <c r="O36" t="str">
         <f t="shared" si="12"/>
-        <v>00</v>
+        <v>02</v>
       </c>
       <c r="P36" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2386,7 +2377,7 @@
       </c>
       <c r="S36" t="str">
         <f t="shared" si="3"/>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="T36" s="1" t="str">
         <f t="shared" si="16"/>
@@ -2394,27 +2385,25 @@
       </c>
       <c r="U36" t="str">
         <f t="shared" si="4"/>
-        <v>ld</v>
+        <v>nop</v>
       </c>
       <c r="V36" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W36" t="str">
+      <c r="W36">
         <f t="shared" si="5"/>
-        <v>AC</v>
+        <v>0</v>
       </c>
       <c r="X36" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y36" t="str">
+      <c r="Y36">
         <f t="shared" si="6"/>
-        <v>D</v>
-      </c>
-      <c r="AD36" s="1" t="s">
-        <v>95</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AD36" s="1"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37">
@@ -2422,20 +2411,11 @@
         <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" t="s">
-        <v>120</v>
-      </c>
-      <c r="D37" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="G37">
         <f t="shared" si="7"/>
-        <v>192</v>
+        <v>2</v>
       </c>
       <c r="H37">
         <f t="shared" si="8"/>
@@ -2443,11 +2423,11 @@
       </c>
       <c r="I37">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J37">
         <f t="shared" si="2"/>
-        <v>194</v>
+        <v>2</v>
       </c>
       <c r="L37" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2463,7 +2443,7 @@
       </c>
       <c r="O37" t="str">
         <f t="shared" si="12"/>
-        <v>C2</v>
+        <v>02</v>
       </c>
       <c r="P37" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2479,7 +2459,7 @@
       </c>
       <c r="S37" t="str">
         <f t="shared" si="3"/>
-        <v>03</v>
+        <v>00</v>
       </c>
       <c r="T37" s="1" t="str">
         <f t="shared" si="16"/>
@@ -2487,27 +2467,25 @@
       </c>
       <c r="U37" t="str">
         <f t="shared" si="4"/>
-        <v>st</v>
+        <v>nop</v>
       </c>
       <c r="V37" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W37" t="str">
+      <c r="W37">
         <f t="shared" si="5"/>
-        <v>[80,D]</v>
+        <v>0</v>
       </c>
       <c r="X37" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y37" t="str">
+      <c r="Y37">
         <f t="shared" si="6"/>
-        <v>AC</v>
-      </c>
-      <c r="Z37" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38">
@@ -2515,11 +2493,11 @@
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
       <c r="G38">
         <f t="shared" si="7"/>
-        <v>227</v>
+        <v>2</v>
       </c>
       <c r="H38">
         <f t="shared" si="8"/>
@@ -2531,7 +2509,7 @@
       </c>
       <c r="J38">
         <f t="shared" si="2"/>
-        <v>227</v>
+        <v>2</v>
       </c>
       <c r="L38" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2547,7 +2525,7 @@
       </c>
       <c r="O38" t="str">
         <f t="shared" si="12"/>
-        <v>E3</v>
+        <v>02</v>
       </c>
       <c r="P38" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2571,7 +2549,7 @@
       </c>
       <c r="U38" t="str">
         <f t="shared" si="4"/>
-        <v>reti</v>
+        <v>nop</v>
       </c>
       <c r="V38" s="1" t="str">
         <f t="shared" si="17"/>
@@ -2589,12 +2567,8 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Z38" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD38" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="Z38" s="1"/>
+      <c r="AD38" s="1"/>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -2602,20 +2576,11 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="G39">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H39">
         <f t="shared" si="8"/>
@@ -2627,7 +2592,7 @@
       </c>
       <c r="J39">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L39" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2643,7 +2608,7 @@
       </c>
       <c r="O39" t="str">
         <f t="shared" si="12"/>
-        <v>00</v>
+        <v>02</v>
       </c>
       <c r="P39" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2667,29 +2632,23 @@
       </c>
       <c r="U39" t="str">
         <f>B39</f>
-        <v>ld</v>
+        <v>nop</v>
       </c>
       <c r="V39" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W39" t="str">
+      <c r="W39">
         <f>C39</f>
-        <v>AC</v>
+        <v>0</v>
       </c>
       <c r="X39" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y39" t="str">
+      <c r="Y39">
         <f>D39</f>
-        <v>D</v>
-      </c>
-      <c r="Z39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD39" s="1" t="s">
-        <v>126</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
@@ -2698,7 +2657,7 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G40">
         <f t="shared" si="7"/>
@@ -2772,7 +2731,6 @@
         <f>D40</f>
         <v>0</v>
       </c>
-      <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -2780,24 +2738,15 @@
         <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="G41">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H41">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I41">
         <f>_xlfn.XLOOKUP(D41,$H$3:$H$7,$I$3:$I$7)</f>
@@ -2805,7 +2754,7 @@
       </c>
       <c r="J41">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="L41" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2821,7 +2770,7 @@
       </c>
       <c r="O41" t="str">
         <f t="shared" si="12"/>
-        <v>14</v>
+        <v>02</v>
       </c>
       <c r="P41" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2845,23 +2794,23 @@
       </c>
       <c r="U41" t="str">
         <f>B41</f>
-        <v>ld</v>
+        <v>nop</v>
       </c>
       <c r="V41" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W41" t="str">
+      <c r="W41">
         <f>C41</f>
-        <v>Y</v>
+        <v>0</v>
       </c>
       <c r="X41" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y41" t="str">
+      <c r="Y41">
         <f>D41</f>
-        <v>D</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
@@ -2870,20 +2819,11 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" t="s">
-        <v>86</v>
-      </c>
-      <c r="D42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="G42">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H42">
         <f t="shared" si="8"/>
@@ -2891,11 +2831,11 @@
       </c>
       <c r="I42">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L42" s="1" t="str">
         <f t="shared" si="9"/>
@@ -2911,7 +2851,7 @@
       </c>
       <c r="O42" t="str">
         <f t="shared" si="12"/>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="P42" s="1" t="str">
         <f t="shared" si="13"/>
@@ -2935,29 +2875,23 @@
       </c>
       <c r="U42" t="str">
         <f t="shared" si="4"/>
-        <v>ld</v>
+        <v>nop</v>
       </c>
       <c r="V42" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W42" t="str">
+      <c r="W42">
         <f t="shared" si="5"/>
-        <v>[80,D],AC</v>
+        <v>0</v>
       </c>
       <c r="X42" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y42" t="str">
+      <c r="Y42">
         <f t="shared" si="6"/>
-        <v>MEM</v>
-      </c>
-      <c r="Z42" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AD42" s="1" t="s">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.25">
@@ -2966,7 +2900,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G43">
         <f t="shared" si="7"/>
@@ -3040,7 +2974,6 @@
         <f>D43</f>
         <v>0</v>
       </c>
-      <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -3048,32 +2981,23 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" t="s">
-        <v>89</v>
-      </c>
-      <c r="D44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="G44">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H44">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I44">
         <f>_xlfn.XLOOKUP(D44,$H$3:$H$7,$I$3:$I$7)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="L44" s="1" t="str">
         <f t="shared" si="9"/>
@@ -3089,7 +3013,7 @@
       </c>
       <c r="O44" t="str">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>02</v>
       </c>
       <c r="P44" s="1" t="str">
         <f t="shared" si="13"/>
@@ -3105,7 +3029,7 @@
       </c>
       <c r="S44" t="str">
         <f>DEC2HEX(E44,2)</f>
-        <v>02</v>
+        <v>00</v>
       </c>
       <c r="T44" s="1" t="str">
         <f t="shared" si="16"/>
@@ -3113,26 +3037,23 @@
       </c>
       <c r="U44" t="str">
         <f>B44</f>
-        <v>ld</v>
+        <v>nop</v>
       </c>
       <c r="V44" s="1" t="str">
         <f t="shared" si="17"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W44" t="str">
+      <c r="W44">
         <f>C44</f>
-        <v>[80,D],Y</v>
+        <v>0</v>
       </c>
       <c r="X44" s="1" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="Y44" t="str">
+      <c r="Y44">
         <f>D44</f>
-        <v>MEM</v>
-      </c>
-      <c r="Z44" s="1" t="s">
-        <v>112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
@@ -3141,11 +3062,11 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
       <c r="G45">
         <f t="shared" si="7"/>
-        <v>227</v>
+        <v>2</v>
       </c>
       <c r="H45">
         <f t="shared" si="8"/>
@@ -3157,7 +3078,7 @@
       </c>
       <c r="J45">
         <f t="shared" si="2"/>
-        <v>227</v>
+        <v>2</v>
       </c>
       <c r="L45" s="1" t="str">
         <f t="shared" si="9"/>
@@ -3173,7 +3094,7 @@
       </c>
       <c r="O45" t="str">
         <f t="shared" si="12"/>
-        <v>E3</v>
+        <v>02</v>
       </c>
       <c r="P45" s="1" t="str">
         <f t="shared" si="13"/>
@@ -3197,7 +3118,7 @@
       </c>
       <c r="U45" t="str">
         <f>B45</f>
-        <v>reti</v>
+        <v>nop</v>
       </c>
       <c r="V45" s="1" t="str">
         <f t="shared" si="17"/>
@@ -3214,9 +3135,6 @@
       <c r="Y45">
         <f>D45</f>
         <v>0</v>
-      </c>
-      <c r="Z45" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.25">
@@ -3310,7 +3228,7 @@
       </c>
       <c r="Z46" s="1"/>
       <c r="AD46" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
@@ -3322,7 +3240,7 @@
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D47" t="s">
         <v>19</v>
@@ -3403,7 +3321,7 @@
         <v>AC</v>
       </c>
       <c r="Z47" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.25">
@@ -3496,10 +3414,10 @@
         <v>D</v>
       </c>
       <c r="Z48" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AD48" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
@@ -3511,7 +3429,7 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D49" t="s">
         <v>19</v>
@@ -3592,10 +3510,10 @@
         <v>AC</v>
       </c>
       <c r="Z49" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AD49" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.25">
@@ -3607,7 +3525,7 @@
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D50" t="s">
         <v>20</v>
@@ -3688,7 +3606,7 @@
         <v>MEM</v>
       </c>
       <c r="Z50" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.25">
@@ -3781,7 +3699,7 @@
         <v>D</v>
       </c>
       <c r="Z51" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
@@ -3793,7 +3711,7 @@
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D52" t="s">
         <v>19</v>
@@ -3871,7 +3789,7 @@
         <v>AC</v>
       </c>
       <c r="Z52" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
@@ -3961,7 +3879,7 @@
         <v>D</v>
       </c>
       <c r="Z53" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add assembler ruleset for instruction set
</commit_message>
<xml_diff>
--- a/resources/Assembly.xlsx
+++ b/resources/Assembly.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\gtxl\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B45A2D1-A803-457B-8BA8-949FE421C09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8EBF04-B533-442D-84F3-CF1DF392156F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-5625" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67080" yWindow="-5625" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="fibon" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="188">
   <si>
     <t>ld</t>
   </si>
@@ -420,6 +421,189 @@
   <si>
     <t>y</t>
   </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>CONTENT</t>
+  </si>
+  <si>
+    <t>BEGIN</t>
+  </si>
+  <si>
+    <t>DEPTH</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>WIDTH</t>
+  </si>
+  <si>
+    <t>ADDRESS_RADIX</t>
+  </si>
+  <si>
+    <t>HEX</t>
+  </si>
+  <si>
+    <t>DATA_RADIX</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>1E</t>
+  </si>
+  <si>
+    <t>1F</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>",</t>
+  </si>
 </sst>
 </file>
 
@@ -454,9 +638,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23:AD53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14151,9 +14336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED5C3B6-8951-4E2A-B650-0DF7E3F63672}">
   <dimension ref="A2:Z106"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19205,4 +19388,1161 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DB438F-FB46-4CB6-96BF-2772BB2DDFFB}">
+  <dimension ref="B1:X47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9">
+        <f>HEX2DEC(C9)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f>D9</f>
+        <v>C2</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="X9" s="1"/>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f t="shared" ref="F10:F46" si="0">F9</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G10">
+        <f>HEX2DEC(C10)</f>
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="str">
+        <f t="shared" ref="H10:H46" si="1">H9</f>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <f t="shared" ref="I10:I46" si="2">D10</f>
+        <v>00</v>
+      </c>
+      <c r="J10" s="1" t="str">
+        <f t="shared" ref="J10:J46" si="3">J9</f>
+        <v>",</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G46" si="4">HEX2DEC(C11)</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>C3</v>
+      </c>
+      <c r="J11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="H12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>01</v>
+      </c>
+      <c r="J12" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I13" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="J13" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="J14" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="H15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>01</v>
+      </c>
+      <c r="J15" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="H16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>03</v>
+      </c>
+      <c r="J16" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="H17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="J17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="J18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>EC</v>
+      </c>
+      <c r="J19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="J20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="H21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="J21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="H22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="J22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="H23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I23" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="J23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="H24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I24" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="J24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="H25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I25" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>01</v>
+      </c>
+      <c r="J25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="H26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I26" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="J26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="H27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I27" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="J27" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="H28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I28" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>01</v>
+      </c>
+      <c r="J28" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="H29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I29" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>E3</v>
+      </c>
+      <c r="J29" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="H30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I30" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="J30" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="H31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I31" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="J31" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="H32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I32" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="J32" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="H33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I33" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>C2</v>
+      </c>
+      <c r="J33" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="H34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I34" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>03</v>
+      </c>
+      <c r="J34" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="H35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I35" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="J35" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="H36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I36" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="J36" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="H37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I37" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>C2</v>
+      </c>
+      <c r="J37" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="H38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I38" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>04</v>
+      </c>
+      <c r="J38" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="H39" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I39" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>01</v>
+      </c>
+      <c r="J39" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="H40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I40" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>04</v>
+      </c>
+      <c r="J40" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="H41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I41" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="J41" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="H42" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I42" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>01</v>
+      </c>
+      <c r="J42" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C43" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="H43" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I43" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1A</v>
+      </c>
+      <c r="J43" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="H44" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I44" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="J44" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="H45" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I45" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>FC</v>
+      </c>
+      <c r="J45" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="H46" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> =&gt;x"</v>
+      </c>
+      <c r="I46" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>1C</v>
+      </c>
+      <c r="J46" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>",</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>